<commit_message>
add export activity export xls file
</commit_message>
<xml_diff>
--- a/src/main/resources/template/BC_ACTIVITY_DOCUMENT.xlsx
+++ b/src/main/resources/template/BC_ACTIVITY_DOCUMENT.xlsx
@@ -5,31 +5,31 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sangvn1\openkm\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0134B330-D744-4BFF-B666-49A612332E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF01E92-4DD3-4222-B335-C1D48AB53389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Table 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Table 5" sheetId="5" r:id="rId5"/>
-    <sheet name="Table 6" sheetId="6" r:id="rId6"/>
-    <sheet name="Table 7" sheetId="7" r:id="rId7"/>
-    <sheet name="Table 8" sheetId="8" r:id="rId8"/>
-    <sheet name="Table 9" sheetId="9" r:id="rId9"/>
-    <sheet name="Table 10" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <r>
       <rPr>
@@ -273,7 +273,12 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">    Căn cứ số liệu trên phần mềm, … (</t>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">     (C</t>
     </r>
     <r>
       <rPr>
@@ -282,7 +287,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">Tên đơn vị của user) </t>
+      <t>hi tiết như phụ lục đính kèm</t>
     </r>
     <r>
       <rPr>
@@ -290,17 +295,13 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>báo cáo Ban Giám đốc  Viện  về  tình  hình  cập  nhật  tài  liệu  ngày  từ  ngày  ${fromDate}  đến  ngày ${toDate}, cụ thể như sau:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">     (C</t>
+      <t>)
+     Trên đây là báo cáo tình hình cập nhật tài liệu của các đơn vị, kính trình Ban Giám đốc Viện xem xét.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Căn cứ số liệu trên phần mềm, ${orgName}</t>
     </r>
     <r>
       <rPr>
@@ -309,7 +310,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>hi tiết như phụ lục đính kèm</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -317,16 +318,54 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>)
-     Trên đây là báo cáo tình hình cập nhật tài liệu của các đơn vị, kính trình Ban Giám đốc Viện xem xét.</t>
-    </r>
+      <t>báo cáo Ban Giám đốc Viện về tình  hình  cập  nhật  tài  liệu  ngày  từ  ngày  ${fromDate} đến ngày ${toDate}, cụ thể như sau:</t>
+    </r>
+  </si>
+  <si>
+    <t>${bean.orgName}</t>
+  </si>
+  <si>
+    <t>${bean.documentName}</t>
+  </si>
+  <si>
+    <t>${bean.action}</t>
+  </si>
+  <si>
+    <t>&lt;/jx:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${bean.index}</t>
+  </si>
+  <si>
+    <t>${bean.fullName}</t>
+  </si>
+  <si>
+    <t>${bean.employeeCode}</t>
+  </si>
+  <si>
+    <t>${bean.dateTime}</t>
+  </si>
+  <si>
+    <t>TỔNG</t>
+  </si>
+  <si>
+    <t>${totalDoc}</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${generalBeans}" var="bean"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${detailBeans}" var="bean"&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
+  </numFmts>
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -407,6 +446,19 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -419,12 +471,64 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -437,46 +541,7 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -487,9 +552,38 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -500,68 +594,123 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -587,7 +736,7 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>524002</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>392288</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1981200" cy="0"/>
@@ -635,10 +784,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>889000</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>515620</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>401813</xdr:rowOff>
+      <xdr:rowOff>409433</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1123950" cy="0"/>
     <xdr:sp macro="" textlink="">
@@ -654,7 +803,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="988060" y="409433"/>
           <a:ext cx="1123950" cy="0"/>
         </a:xfrm>
         <a:custGeom>
@@ -685,10 +834,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2098675</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>628015</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>453931</xdr:rowOff>
+      <xdr:rowOff>469171</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1936114" cy="635"/>
     <xdr:sp macro="" textlink="">
@@ -704,7 +853,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2098675" y="453931"/>
+          <a:off x="2449195" y="1322611"/>
           <a:ext cx="1936114" cy="635"/>
         </a:xfrm>
         <a:custGeom>
@@ -1057,354 +1206,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="3" spans="1:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+    </row>
+    <row r="4" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="103.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+    </row>
+    <row r="6" spans="1:8" ht="103.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
+    </row>
+    <row r="8" spans="1:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="16" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="22" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="24" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="14" t="s">
+      <c r="F24" s="17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="13" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="19" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="21" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="G24" s="18" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="19"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="C9:E9"/>
+  <mergeCells count="13">
+    <mergeCell ref="A8:F8"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="30.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="112" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="112" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="105.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="129.44999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="112" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="112" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="54" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="112" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove org field add doc
</commit_message>
<xml_diff>
--- a/src/main/resources/template/BC_ACTIVITY_DOCUMENT.xlsx
+++ b/src/main/resources/template/BC_ACTIVITY_DOCUMENT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sangvn1\openkm\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD7A91D-D38E-439F-B50B-27E576B0387E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF29153-A65E-4564-B516-17B57F5989A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Số:         /${orgCode}</t>
+      <t>Số:         /${orgCode}-BC</t>
     </r>
   </si>
 </sst>
@@ -672,12 +672,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -695,21 +710,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1222,7 +1222,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="26"/>
@@ -1244,24 +1244,24 @@
       <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="103.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="8" spans="1:8" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
@@ -1280,11 +1280,11 @@
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1306,11 +1306,11 @@
       <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="12" t="s">
         <v>18</v>
       </c>
@@ -1334,11 +1334,11 @@
         <v>24</v>
       </c>
       <c r="B13" s="9"/>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="13"/>
       <c r="G13" s="5"/>
       <c r="H13" s="1"/>
@@ -1359,11 +1359,11 @@
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="22" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
@@ -1446,12 +1446,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:F6"/>
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:F16"/>
@@ -1459,6 +1453,12 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>